<commit_message>
Before changing root segment age...
</commit_message>
<xml_diff>
--- a/simulations/running_scenarios/inputs/scenarios_list.xlsx
+++ b/simulations/running_scenarios/inputs/scenarios_list.xlsx
@@ -2402,10 +2402,10 @@
   <dimension ref="A1:XEM160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="H149" sqref="H149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2638,13 +2638,13 @@
         <v>5.0000000000000001E-9</v>
       </c>
       <c r="E10" s="79">
-        <v>5.0000000000000001E-9</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="F10" s="79">
-        <v>5.0000000000000001E-9</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="G10" s="79">
-        <v>5.0000000000000001E-9</v>
+        <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -71530,9 +71530,15 @@
       <c r="D160" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="E160" s="84"/>
-      <c r="F160" s="84"/>
-      <c r="G160" s="84"/>
+      <c r="E160" s="84">
+        <v>8</v>
+      </c>
+      <c r="F160" s="84">
+        <v>9</v>
+      </c>
+      <c r="G160" s="84">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commit before modifying plotting functions
</commit_message>
<xml_diff>
--- a/simulations/running_scenarios/inputs/scenarios_list.xlsx
+++ b/simulations/running_scenarios/inputs/scenarios_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="479">
   <si>
     <t>input_file</t>
   </si>
@@ -1448,7 +1448,16 @@
     <t xml:space="preserve">Time in the input file at which the simulation will start </t>
   </si>
   <si>
-    <t>sucrose_input_0047.csv</t>
+    <t>C_hexose_min_for_elongation</t>
+  </si>
+  <si>
+    <t>C_hexose_min_for_thickening</t>
+  </si>
+  <si>
+    <t>Treshold hexose concentration for elongation, below which no elongation occurs</t>
+  </si>
+  <si>
+    <t>Treshold hexose concentration for elongation, below which no thickening occurs</t>
   </si>
 </sst>
 </file>
@@ -1610,7 +1619,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="56">
+  <fills count="54">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1894,12 +1903,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1919,12 +1922,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2104,7 +2101,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2270,45 +2267,36 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="52" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="11" fontId="0" fillId="50" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="50" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="50" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="50" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="53" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="51" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="51" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="51" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="51" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="53" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="53" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="53" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="51" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="51" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="54" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="54" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="54" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="55" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="51" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2683,7 +2671,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E192"/>
+  <dimension ref="A1:F194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -2698,10 +2686,11 @@
     <col min="2" max="2" width="64.77734375" customWidth="1"/>
     <col min="3" max="3" width="19.88671875" customWidth="1"/>
     <col min="4" max="4" width="17" style="46" customWidth="1"/>
-    <col min="5" max="14" width="15.77734375" customWidth="1"/>
+    <col min="5" max="6" width="15.77734375" style="46" customWidth="1"/>
+    <col min="7" max="11" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>95</v>
       </c>
@@ -2715,10 +2704,13 @@
         <v>389</v>
       </c>
       <c r="E1" s="44">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="F1" s="44">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2734,8 +2726,11 @@
       <c r="E2" s="39" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2751,42 +2746,51 @@
       <c r="E3" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="90" t="s">
+      <c r="F3" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="89" t="s">
         <v>466</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="90" t="s">
         <v>468</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="90" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="91" t="s">
         <v>88</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="90" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="89" t="s">
         <v>467</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="90" t="s">
         <v>469</v>
       </c>
-      <c r="C5" s="91" t="s">
+      <c r="C5" s="90" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="92" t="s">
+      <c r="D5" s="91" t="s">
         <v>470</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="39" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -2799,11 +2803,14 @@
       <c r="D6" s="64">
         <v>60</v>
       </c>
-      <c r="E6" s="82">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="81">
+        <v>180</v>
+      </c>
+      <c r="F6" s="81">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -2819,8 +2826,11 @@
       <c r="E7" s="40">
         <v>4.1666666999999998E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="40">
+        <v>4.1666666999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -2833,11 +2843,16 @@
       <c r="D8" s="64">
         <v>5</v>
       </c>
-      <c r="E8" s="96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="94">
+        <f>E7</f>
+        <v>4.1666666999999998E-2</v>
+      </c>
+      <c r="F8" s="94">
+        <f>F7</f>
+        <v>4.1666666999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
@@ -2851,10 +2866,13 @@
         <v>86</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -2868,11 +2886,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="39">
-        <f t="shared" ref="E10" si="0">1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>473</v>
       </c>
@@ -2885,11 +2905,14 @@
       <c r="D11" s="62">
         <v>0</v>
       </c>
-      <c r="E11" s="95">
+      <c r="E11" s="93">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
@@ -2902,11 +2925,14 @@
       <c r="D12" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="97" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
@@ -2919,11 +2945,14 @@
       <c r="D13" s="50">
         <v>5.0000000000000001E-9</v>
       </c>
-      <c r="E13" s="84">
+      <c r="E13" s="41">
         <v>5.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="41">
+        <v>5.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
@@ -2936,11 +2965,14 @@
       <c r="D14" s="62">
         <v>10</v>
       </c>
-      <c r="E14" s="97">
+      <c r="E14" s="39">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>10</v>
       </c>
@@ -2956,8 +2988,11 @@
       <c r="E15" s="39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>11</v>
       </c>
@@ -2973,8 +3008,11 @@
       <c r="E16" s="39">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>373</v>
       </c>
@@ -2987,11 +3025,14 @@
       <c r="D17" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="89" t="s">
+      <c r="E17" s="88" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="88" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>375</v>
       </c>
@@ -3007,8 +3048,11 @@
       <c r="E18" s="47" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>387</v>
       </c>
@@ -3024,8 +3068,11 @@
       <c r="E19" s="39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>386</v>
       </c>
@@ -3041,8 +3088,11 @@
       <c r="E20" s="47" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>385</v>
       </c>
@@ -3058,8 +3108,11 @@
       <c r="E21" s="47" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>12</v>
       </c>
@@ -3075,8 +3128,11 @@
       <c r="E22" s="39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>13</v>
       </c>
@@ -3092,8 +3148,11 @@
       <c r="E23" s="39">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="39">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>14</v>
       </c>
@@ -3109,8 +3168,11 @@
       <c r="E24" s="39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>9</v>
       </c>
@@ -3126,8 +3188,11 @@
       <c r="E25" s="39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
         <v>21</v>
       </c>
@@ -3143,8 +3208,11 @@
       <c r="E26" s="39" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>22</v>
       </c>
@@ -3160,8 +3228,11 @@
       <c r="E27" s="39" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="39" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>23</v>
       </c>
@@ -3177,8 +3248,11 @@
       <c r="E28" s="41">
         <v>9.9999999999999995E-7</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="41">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
         <v>24</v>
       </c>
@@ -3194,8 +3268,11 @@
       <c r="E29" s="41">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" s="41">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>25</v>
       </c>
@@ -3211,8 +3288,11 @@
       <c r="E30" s="39" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>26</v>
       </c>
@@ -3228,8 +3308,11 @@
       <c r="E31" s="39" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" s="39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>27</v>
       </c>
@@ -3245,8 +3328,11 @@
       <c r="E32" s="39" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>28</v>
       </c>
@@ -3262,8 +3348,11 @@
       <c r="E33" s="39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>29</v>
       </c>
@@ -3279,8 +3368,11 @@
       <c r="E34" s="39">
         <v>120</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" s="39">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>30</v>
       </c>
@@ -3296,8 +3388,11 @@
       <c r="E35" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>31</v>
       </c>
@@ -3313,8 +3408,11 @@
       <c r="E36" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
         <v>32</v>
       </c>
@@ -3330,8 +3428,11 @@
       <c r="E37" s="39">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" s="39">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
         <v>33</v>
       </c>
@@ -3347,8 +3448,11 @@
       <c r="E38" s="39">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" s="39">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
         <v>34</v>
       </c>
@@ -3364,8 +3468,11 @@
       <c r="E39" s="39">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" s="39">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
         <v>35</v>
       </c>
@@ -3381,8 +3488,11 @@
       <c r="E40" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
         <v>449</v>
       </c>
@@ -3398,8 +3508,11 @@
       <c r="E41" s="39">
         <v>1200</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41" s="39">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>450</v>
       </c>
@@ -3415,8 +3528,11 @@
       <c r="E42" s="39">
         <v>1200</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42" s="39">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
         <v>15</v>
       </c>
@@ -3432,8 +3548,11 @@
       <c r="E43" s="39" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>16</v>
       </c>
@@ -3449,8 +3568,11 @@
       <c r="E44" s="39" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
         <v>17</v>
       </c>
@@ -3466,8 +3588,11 @@
       <c r="E45" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
         <v>18</v>
       </c>
@@ -3483,8 +3608,11 @@
       <c r="E46" s="39">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46" s="39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>19</v>
       </c>
@@ -3500,8 +3628,11 @@
       <c r="E47" s="39">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47" s="39">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
         <v>36</v>
       </c>
@@ -3517,8 +3648,11 @@
       <c r="E48" s="41">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" s="41">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="16" t="s">
         <v>390</v>
       </c>
@@ -3534,8 +3668,11 @@
       <c r="E49" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
         <v>37</v>
       </c>
@@ -3551,8 +3688,11 @@
       <c r="E50" s="39">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50" s="39">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="16" t="s">
         <v>38</v>
       </c>
@@ -3568,8 +3708,11 @@
       <c r="E51" s="39">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51" s="39">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="18" t="s">
         <v>39</v>
       </c>
@@ -3585,8 +3728,11 @@
       <c r="E52" s="39">
         <v>6.9999999999999999E-4</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52" s="39">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
         <v>40</v>
       </c>
@@ -3602,8 +3748,11 @@
       <c r="E53" s="39">
         <v>1.22E-4</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53" s="39">
+        <v>1.22E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="18" t="s">
         <v>217</v>
       </c>
@@ -3619,8 +3768,11 @@
       <c r="E54" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
         <v>41</v>
       </c>
@@ -3636,8 +3788,11 @@
       <c r="E55" s="39">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55" s="39">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
         <v>418</v>
       </c>
@@ -3653,8 +3808,11 @@
       <c r="E56" s="39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
         <v>91</v>
       </c>
@@ -3670,8 +3828,11 @@
       <c r="E57" s="39">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
         <v>420</v>
       </c>
@@ -3687,8 +3848,11 @@
       <c r="E58" s="39" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58" s="39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="18" t="s">
         <v>42</v>
       </c>
@@ -3704,8 +3868,11 @@
       <c r="E59" s="39">
         <v>50</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59" s="39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="18" t="s">
         <v>218</v>
       </c>
@@ -3721,8 +3888,11 @@
       <c r="E60" s="40">
         <v>1453890.8941884842</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60" s="40">
+        <v>1453890.8941884842</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="18" t="s">
         <v>43</v>
       </c>
@@ -3738,8 +3908,11 @@
       <c r="E61" s="40">
         <v>1.3888888888888888E-5</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61" s="40">
+        <v>1.3888888888888888E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="18" t="s">
         <v>44</v>
       </c>
@@ -3755,8 +3928,11 @@
       <c r="E62" s="40">
         <v>6.5011574074074071E-4</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62" s="40">
+        <v>6.5011574074074071E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="18" t="s">
         <v>45</v>
       </c>
@@ -3772,8 +3948,11 @@
       <c r="E63" s="39">
         <v>4.7400000000000003E-3</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63" s="39">
+        <v>4.7400000000000003E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="18" t="s">
         <v>46</v>
       </c>
@@ -3789,8 +3968,11 @@
       <c r="E64" s="40">
         <v>282528</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64" s="40">
+        <v>282528</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="18" t="s">
         <v>47</v>
       </c>
@@ -3806,8 +3988,11 @@
       <c r="E65" s="39">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65" s="39">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="18" t="s">
         <v>48</v>
       </c>
@@ -3823,8 +4008,11 @@
       <c r="E66" s="80">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66" s="80">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
         <v>49</v>
       </c>
@@ -3840,8 +4028,11 @@
       <c r="E67" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="36" t="s">
         <v>50</v>
       </c>
@@ -3857,8 +4048,11 @@
       <c r="E68" s="40">
         <v>745476480000</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68" s="40">
+        <v>745476480000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="36" t="s">
         <v>215</v>
       </c>
@@ -3874,8 +4068,11 @@
       <c r="E69" s="39">
         <v>100</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="36" t="s">
         <v>426</v>
       </c>
@@ -3891,8 +4088,11 @@
       <c r="E70" s="39" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70" s="39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="36" t="s">
         <v>411</v>
       </c>
@@ -3908,8 +4108,11 @@
       <c r="E71" s="39">
         <v>21600</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71" s="39">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="36" t="s">
         <v>422</v>
       </c>
@@ -3925,8 +4128,11 @@
       <c r="E72" s="39">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72" s="39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="36" t="s">
         <v>412</v>
       </c>
@@ -3942,8 +4148,11 @@
       <c r="E73" s="39">
         <v>60479.999999999993</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73" s="39">
+        <v>60479.999999999993</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="36" t="s">
         <v>423</v>
       </c>
@@ -3959,8 +4168,11 @@
       <c r="E74" s="39">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74" s="39">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="36" t="s">
         <v>413</v>
       </c>
@@ -3976,8 +4188,11 @@
       <c r="E75" s="39">
         <v>518400</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75" s="39">
+        <v>518400</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="36" t="s">
         <v>424</v>
       </c>
@@ -3993,8 +4208,11 @@
       <c r="E76" s="39">
         <v>5184000</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76" s="39">
+        <v>5184000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="18" t="s">
         <v>51</v>
       </c>
@@ -4010,8 +4228,11 @@
       <c r="E77" s="41">
         <v>50000</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77" s="41">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="18" t="s">
         <v>52</v>
       </c>
@@ -4027,8 +4248,11 @@
       <c r="E78" s="39">
         <v>140000</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78" s="39">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="18" t="s">
         <v>53</v>
       </c>
@@ -4044,8 +4268,11 @@
       <c r="E79" s="40">
         <v>3.6636136999999999E-2</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79" s="40">
+        <v>3.6636136999999999E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="18" t="s">
         <v>54</v>
       </c>
@@ -4061,8 +4288,11 @@
       <c r="E80" s="39">
         <v>4.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80" s="39">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="18" t="s">
         <v>55</v>
       </c>
@@ -4078,8 +4308,11 @@
       <c r="E81" s="39">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81" s="39">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="20" t="s">
         <v>224</v>
       </c>
@@ -4095,8 +4328,11 @@
       <c r="E82" s="39">
         <v>6.0000000000000002E-6</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82" s="39">
+        <v>6.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="20" t="s">
         <v>225</v>
       </c>
@@ -4112,8 +4348,11 @@
       <c r="E83" s="39">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83" s="39">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="20" t="s">
         <v>226</v>
       </c>
@@ -4129,8 +4368,11 @@
       <c r="E84" s="39">
         <v>374999999.99999994</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84" s="39">
+        <v>374999999.99999994</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="20" t="s">
         <v>227</v>
       </c>
@@ -4146,8 +4388,11 @@
       <c r="E85" s="40">
         <v>3.7037037037037038E-3</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F85" s="40">
+        <v>3.7037037037037038E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="20" t="s">
         <v>228</v>
       </c>
@@ -4163,8 +4408,11 @@
       <c r="E86" s="39">
         <v>165600</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F86" s="39">
+        <v>165600</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="14" t="s">
         <v>60</v>
       </c>
@@ -4180,8 +4428,11 @@
       <c r="E87" s="39">
         <v>20</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F87" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="14" t="s">
         <v>219</v>
       </c>
@@ -4197,8 +4448,11 @@
       <c r="E88" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F88" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="14" t="s">
         <v>59</v>
       </c>
@@ -4214,8 +4468,11 @@
       <c r="E89" s="39">
         <v>21</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F89" s="39">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="24" t="s">
         <v>65</v>
       </c>
@@ -4231,8 +4488,11 @@
       <c r="E90" s="39">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F90" s="39">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="24" t="s">
         <v>377</v>
       </c>
@@ -4248,8 +4508,11 @@
       <c r="E91" s="39">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91" s="39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="24" t="s">
         <v>378</v>
       </c>
@@ -4265,8 +4528,11 @@
       <c r="E92" s="39">
         <v>10</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="24" t="s">
         <v>379</v>
       </c>
@@ -4282,8 +4548,11 @@
       <c r="E93" s="39">
         <v>8</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93" s="39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="24" t="s">
         <v>394</v>
       </c>
@@ -4299,8 +4568,11 @@
       <c r="E94" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
         <v>396</v>
       </c>
@@ -4316,8 +4588,11 @@
       <c r="E95" s="39">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95" s="39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="24" t="s">
         <v>398</v>
       </c>
@@ -4333,8 +4608,11 @@
       <c r="E96" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="24" t="s">
         <v>400</v>
       </c>
@@ -4350,8 +4628,11 @@
       <c r="E97" s="77">
         <v>1589759.9999999998</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97" s="77">
+        <v>1589759.9999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="24" t="s">
         <v>402</v>
       </c>
@@ -4367,8 +4648,11 @@
       <c r="E98" s="77">
         <v>6171428.5714285718</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98" s="77">
+        <v>6171428.5714285718</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="24" t="s">
         <v>404</v>
       </c>
@@ -4384,8 +4668,11 @@
       <c r="E99" s="77">
         <v>6171428.5714285718</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99" s="77">
+        <v>6171428.5714285718</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="24" t="s">
         <v>433</v>
       </c>
@@ -4401,8 +4688,11 @@
       <c r="E100" s="77">
         <v>100</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F100" s="77">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="24" t="s">
         <v>435</v>
       </c>
@@ -4418,8 +4708,11 @@
       <c r="E101" s="77">
         <v>280800</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F101" s="77">
+        <v>280800</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="24" t="s">
         <v>437</v>
       </c>
@@ -4435,8 +4728,11 @@
       <c r="E102" s="77">
         <v>1.2847222222222224E-5</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F102" s="77">
+        <v>1.2847222222222224E-5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="24" t="s">
         <v>439</v>
       </c>
@@ -4452,8 +4748,11 @@
       <c r="E103" s="77">
         <v>100</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F103" s="77">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="24" t="s">
         <v>441</v>
       </c>
@@ -4469,8 +4768,11 @@
       <c r="E104" s="77">
         <v>459648</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F104" s="77">
+        <v>459648</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="24" t="s">
         <v>443</v>
       </c>
@@ -4486,8 +4788,11 @@
       <c r="E105" s="77">
         <v>1.2847222222222224E-5</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F105" s="77">
+        <v>1.2847222222222224E-5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="24" t="s">
         <v>406</v>
       </c>
@@ -4503,8 +4808,11 @@
       <c r="E106" s="77">
         <v>21600</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F106" s="77">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="24" t="s">
         <v>408</v>
       </c>
@@ -4520,8 +4828,11 @@
       <c r="E107" s="77">
         <v>43200</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F107" s="77">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="14" t="s">
         <v>61</v>
       </c>
@@ -4537,8 +4848,11 @@
       <c r="E108" s="39">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F108" s="39">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
         <v>62</v>
       </c>
@@ -4554,8 +4868,11 @@
       <c r="E109" s="40">
         <v>2.0833333333333335E-4</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F109" s="40">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="14" t="s">
         <v>63</v>
       </c>
@@ -4571,8 +4888,11 @@
       <c r="E110" s="42">
         <v>5.7899999999999998E-7</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F110" s="42">
+        <v>5.7899999999999998E-7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
         <v>64</v>
       </c>
@@ -4588,713 +4908,839 @@
       <c r="E111" s="40">
         <v>2.0833333333333335E-4</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="85" t="s">
+      <c r="F111" s="40">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="B112" s="15" t="s">
+        <v>477</v>
+      </c>
+      <c r="C112" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D112" s="52">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E112" s="40">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F112" s="40">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="B113" s="15" t="s">
+        <v>478</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D113" s="52">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E113" s="40">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F113" s="40">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" s="84" t="s">
         <v>457</v>
       </c>
-      <c r="B112" s="86" t="s">
+      <c r="B114" s="85" t="s">
         <v>189</v>
       </c>
-      <c r="C112" s="86" t="s">
+      <c r="C114" s="85" t="s">
         <v>190</v>
       </c>
-      <c r="D112" s="87">
+      <c r="D114" s="86">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E112" s="84" t="s">
+      <c r="E114" s="92" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A113" s="85" t="s">
+      <c r="F114" s="92" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="B113" s="86" t="s">
+      <c r="B115" s="85" t="s">
         <v>460</v>
       </c>
-      <c r="C113" s="86" t="s">
+      <c r="C115" s="85" t="s">
         <v>461</v>
       </c>
-      <c r="D113" s="88">
+      <c r="D115" s="87">
         <v>1.6666666666666666E-4</v>
       </c>
-      <c r="E113" s="84" t="s">
+      <c r="E115" s="92" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A114" s="85" t="s">
+      <c r="F115" s="92" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="84" t="s">
         <v>471</v>
       </c>
-      <c r="B114" s="86" t="s">
+      <c r="B116" s="85" t="s">
         <v>472</v>
       </c>
-      <c r="C114" s="86" t="s">
+      <c r="C116" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="D114" s="88" t="s">
+      <c r="D116" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="E114" s="94" t="s">
+      <c r="E116" s="92" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A115" s="22" t="s">
+      <c r="F116" s="92" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B115" s="23" t="s">
+      <c r="B117" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="C115" s="23" t="s">
+      <c r="C117" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="D115" s="68">
+      <c r="D117" s="68">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E115" s="81">
+      <c r="E117" s="41">
         <v>5.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A116" s="22" t="s">
+      <c r="F117" s="41">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="22" t="s">
         <v>453</v>
       </c>
-      <c r="B116" s="23" t="s">
+      <c r="B118" s="23" t="s">
         <v>454</v>
       </c>
-      <c r="C116" s="23" t="s">
+      <c r="C118" s="23" t="s">
         <v>455</v>
       </c>
-      <c r="D116" s="78">
+      <c r="D118" s="78">
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="E116" s="83">
+      <c r="E118" s="82">
         <v>2.7799999999999999E-14</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A117" s="22" t="s">
+      <c r="F118" s="82">
+        <v>2.7799999999999999E-14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="22" t="s">
         <v>462</v>
       </c>
-      <c r="B117" s="23" t="s">
+      <c r="B119" s="23" t="s">
         <v>322</v>
       </c>
-      <c r="C117" s="23" t="s">
+      <c r="C119" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="D117" s="68">
+      <c r="D119" s="68">
         <v>10</v>
       </c>
-      <c r="E117" s="39">
+      <c r="E119" s="39">
         <v>10</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A118" s="22" t="s">
+      <c r="F119" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" s="22" t="s">
         <v>463</v>
       </c>
-      <c r="B118" s="23" t="s">
+      <c r="B120" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="C118" s="23" t="s">
+      <c r="C120" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="D118" s="68">
+      <c r="D120" s="68">
         <v>-0.04</v>
       </c>
-      <c r="E118" s="39">
+      <c r="E120" s="39">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A119" s="22" t="s">
+      <c r="F120" s="39">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B119" s="23" t="s">
+      <c r="B121" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="C119" s="23" t="s">
+      <c r="C121" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D119" s="68">
+      <c r="D121" s="68">
         <v>2.9</v>
       </c>
-      <c r="E119" s="39">
+      <c r="E121" s="39">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A120" s="22" t="s">
+      <c r="F121" s="39">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" s="22" t="s">
         <v>465</v>
       </c>
-      <c r="B120" s="23" t="s">
+      <c r="B122" s="23" t="s">
         <v>325</v>
       </c>
-      <c r="C120" s="23" t="s">
+      <c r="C122" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D120" s="68">
+      <c r="D122" s="68">
         <v>1</v>
       </c>
-      <c r="E120" s="39">
+      <c r="E122" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A121" s="85" t="s">
+      <c r="F122" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" s="84" t="s">
         <v>456</v>
       </c>
-      <c r="B121" s="86" t="s">
+      <c r="B123" s="85" t="s">
         <v>458</v>
       </c>
-      <c r="C121" s="86" t="s">
+      <c r="C123" s="85" t="s">
         <v>459</v>
       </c>
-      <c r="D121" s="87">
+      <c r="D123" s="86">
         <v>6.0000000000000002E-5</v>
       </c>
-      <c r="E121" s="41">
+      <c r="E123" s="41">
         <v>1.9999999999999999E-7</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A122" s="22" t="s">
+      <c r="F123" s="41">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="B122" s="23" t="s">
+      <c r="B124" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="C122" s="23" t="s">
+      <c r="C124" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="D122" s="68">
+      <c r="D124" s="68">
         <v>10</v>
       </c>
-      <c r="E122" s="39">
+      <c r="E124" s="39">
         <v>10</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A123" s="22" t="s">
+      <c r="F124" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="B123" s="23" t="s">
+      <c r="B125" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="C123" s="23" t="s">
+      <c r="C125" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="D123" s="68">
+      <c r="D125" s="68">
         <v>-0.04</v>
       </c>
-      <c r="E123" s="39">
+      <c r="E125" s="39">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A124" s="22" t="s">
+      <c r="F125" s="39">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="B124" s="23" t="s">
+      <c r="B126" s="23" t="s">
         <v>328</v>
-      </c>
-      <c r="C124" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D124" s="68">
-        <v>2.9</v>
-      </c>
-      <c r="E124" s="39">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A125" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="B125" s="23" t="s">
-        <v>329</v>
-      </c>
-      <c r="C125" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D125" s="68">
-        <v>1</v>
-      </c>
-      <c r="E125" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A126" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B126" s="23" t="s">
-        <v>191</v>
       </c>
       <c r="C126" s="23" t="s">
         <v>103</v>
       </c>
       <c r="D126" s="68">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E126" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.9</v>
+      </c>
+      <c r="F126" s="39">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="22" t="s">
-        <v>70</v>
+        <v>246</v>
       </c>
       <c r="B127" s="23" t="s">
-        <v>192</v>
+        <v>329</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="D127" s="57">
-        <v>1.6666666666666666E-4</v>
-      </c>
-      <c r="E127" s="84">
-        <v>5.0000000000000004E-6</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A128" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B128" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="C128" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="D128" s="56">
+        <v>98</v>
+      </c>
+      <c r="D127" s="68">
+        <v>1</v>
+      </c>
+      <c r="E127" s="39">
+        <v>1</v>
+      </c>
+      <c r="F127" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B128" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="C128" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D128" s="68">
         <v>0</v>
       </c>
       <c r="E128" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A129" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B129" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="C129" s="25" t="s">
+      <c r="F128" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B129" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="C129" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="D129" s="56">
-        <v>2E-3</v>
-      </c>
-      <c r="E129" s="39">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D129" s="57">
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="E129" s="41">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="F129" s="41">
+        <v>5.0000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B130" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C130" s="25" t="s">
         <v>209</v>
       </c>
       <c r="D130" s="56">
+        <v>0</v>
+      </c>
+      <c r="E130" s="39">
+        <v>0</v>
+      </c>
+      <c r="F130" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B131" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C131" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D131" s="56">
+        <v>2E-3</v>
+      </c>
+      <c r="E131" s="39">
+        <v>2E-3</v>
+      </c>
+      <c r="F131" s="39">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B132" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C132" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D132" s="56">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="E130" s="41">
+      <c r="E132" s="41">
         <v>3.9999999999999998E-6</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A131" s="24" t="s">
+      <c r="F132" s="41">
+        <v>3.9999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B131" s="25" t="s">
+      <c r="B133" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="C131" s="25" t="s">
+      <c r="C133" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="D131" s="56">
+      <c r="D133" s="56">
         <v>3.7699999999999999E-10</v>
       </c>
-      <c r="E131" s="41">
+      <c r="E133" s="41">
         <v>3.7699999999999999E-10</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A132" s="24" t="s">
+      <c r="F133" s="41">
+        <v>3.7699999999999999E-10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="B132" s="25" t="s">
+      <c r="B134" s="25" t="s">
         <v>314</v>
       </c>
-      <c r="C132" s="25" t="s">
+      <c r="C134" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D132" s="56">
+      <c r="D134" s="56">
         <v>20</v>
       </c>
-      <c r="E132" s="39">
+      <c r="E134" s="39">
         <v>20</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A133" s="24" t="s">
+      <c r="F134" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="B133" s="25" t="s">
+      <c r="B135" s="25" t="s">
         <v>315</v>
       </c>
-      <c r="C133" s="25" t="s">
+      <c r="C135" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="D133" s="56">
+      <c r="D135" s="56">
         <v>-0.06</v>
       </c>
-      <c r="E133" s="39">
+      <c r="E135" s="39">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A134" s="24" t="s">
+      <c r="F135" s="39">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="B134" s="25" t="s">
+      <c r="B136" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="C134" s="25" t="s">
+      <c r="C136" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="D134" s="56">
+      <c r="D136" s="56">
         <v>0.89100000000000001</v>
       </c>
-      <c r="E134" s="39">
+      <c r="E136" s="39">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A135" s="24" t="s">
+      <c r="F136" s="39">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="B135" s="25" t="s">
+      <c r="B137" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="C135" s="25" t="s">
+      <c r="C137" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D135" s="56">
+      <c r="D137" s="56">
         <v>1</v>
       </c>
-      <c r="E135" s="39">
+      <c r="E137" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A136" s="24" t="s">
+      <c r="F137" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B136" s="25" t="s">
+      <c r="B138" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="C136" s="25" t="s">
+      <c r="C138" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="D136" s="56">
+      <c r="D138" s="56">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="E136" s="41">
+      <c r="E138" s="41">
         <v>4.0000000000000003E-5</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A137" s="14" t="s">
+      <c r="F138" s="41">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B137" s="15" t="s">
+      <c r="B139" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="C137" s="15" t="s">
+      <c r="C139" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="D137" s="52">
+      <c r="D139" s="52">
         <v>5.8333333333333335E-9</v>
       </c>
-      <c r="E137" s="41">
+      <c r="E139" s="41">
         <v>5.8333333333333335E-9</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A138" s="14" t="s">
+      <c r="F139" s="41">
+        <v>5.8333333333333335E-9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="B138" s="15" t="s">
+      <c r="B140" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="C138" s="15" t="s">
+      <c r="C140" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D138" s="61">
+      <c r="D140" s="61">
         <v>20</v>
       </c>
-      <c r="E138" s="39">
+      <c r="E140" s="39">
         <v>20</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A139" s="14" t="s">
+      <c r="F140" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="B139" s="15" t="s">
+      <c r="B141" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="C139" s="15" t="s">
+      <c r="C141" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="D139" s="61">
+      <c r="D141" s="61">
         <v>-0.06</v>
       </c>
-      <c r="E139" s="39">
+      <c r="E141" s="39">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A140" s="14" t="s">
+      <c r="F141" s="39">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="B140" s="15" t="s">
+      <c r="B142" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="C140" s="15" t="s">
+      <c r="C142" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D140" s="61">
+      <c r="D142" s="61">
         <v>0.89100000000000001</v>
       </c>
-      <c r="E140" s="39">
+      <c r="E142" s="39">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A141" s="14" t="s">
+      <c r="F142" s="39">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="B141" s="15" t="s">
+      <c r="B143" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="C141" s="15" t="s">
+      <c r="C143" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D141" s="61">
+      <c r="D143" s="61">
         <v>1</v>
       </c>
-      <c r="E141" s="39">
+      <c r="E143" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A142" s="14" t="s">
+      <c r="F143" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B142" s="15" t="s">
+      <c r="B144" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="C142" s="15" t="s">
+      <c r="C144" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="D142" s="61">
+      <c r="D144" s="61">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="E142" s="41">
+      <c r="E144" s="41">
         <v>4.0000000000000003E-5</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A143" s="10" t="s">
+      <c r="F144" s="41">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B143" s="11" t="s">
+      <c r="B145" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="C143" s="11" t="s">
+      <c r="C145" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="D143" s="51">
+      <c r="D145" s="51">
         <v>4.9999999999999998E-8</v>
       </c>
-      <c r="E143" s="84">
+      <c r="E145" s="83">
         <v>9.9999999999999995E-8</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A144" s="10" t="s">
+      <c r="F145" s="83">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="B144" s="11" t="s">
+      <c r="B146" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="C144" s="11" t="s">
+      <c r="C146" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D144" s="63">
+      <c r="D146" s="63">
         <v>20</v>
       </c>
-      <c r="E144" s="39">
+      <c r="E146" s="39">
         <v>20</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A145" s="10" t="s">
+      <c r="F146" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="B145" s="11" t="s">
+      <c r="B147" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="C145" s="11" t="s">
+      <c r="C147" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="D145" s="63">
+      <c r="D147" s="63">
         <v>-4.4200000000000003E-2</v>
       </c>
-      <c r="E145" s="39">
+      <c r="E147" s="39">
         <v>-4.4200000000000003E-2</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A146" s="10" t="s">
+      <c r="F147" s="39">
+        <v>-4.4200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="B146" s="11" t="s">
+      <c r="B148" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="C146" s="11" t="s">
+      <c r="C148" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D146" s="63">
+      <c r="D148" s="63">
         <v>1.55</v>
       </c>
-      <c r="E146" s="39">
+      <c r="E148" s="39">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A147" s="10" t="s">
+      <c r="F148" s="39">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="B147" s="11" t="s">
+      <c r="B149" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="C147" s="11" t="s">
+      <c r="C149" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D147" s="63">
+      <c r="D149" s="63">
         <v>1</v>
       </c>
-      <c r="E147" s="39">
+      <c r="E149" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A148" s="10" t="s">
+      <c r="F149" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B148" s="11" t="s">
+      <c r="B150" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C148" s="11" t="s">
+      <c r="C150" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="D148" s="63">
+      <c r="D150" s="63">
         <v>2.7799999999999998E-4</v>
       </c>
-      <c r="E148" s="39">
+      <c r="E150" s="39">
         <v>2.7799999999999998E-4</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A149" s="26" t="s">
+      <c r="F150" s="39">
+        <v>2.7799999999999998E-4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B149" s="27" t="s">
+      <c r="B151" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="C149" s="27" t="s">
+      <c r="C151" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="D149" s="73">
+      <c r="D151" s="73">
         <v>6.3200000000000001E-3</v>
       </c>
-      <c r="E149" s="93">
+      <c r="E151" s="41">
         <v>2.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A150" s="26" t="s">
+      <c r="F151" s="41">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="B150" s="27" t="s">
+      <c r="B152" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="C150" s="27" t="s">
+      <c r="C152" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="D150" s="73">
+      <c r="D152" s="73">
         <v>20</v>
       </c>
-      <c r="E150" s="39">
+      <c r="E152" s="39">
         <v>20</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A151" s="26" t="s">
+      <c r="F152" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="B151" s="27" t="s">
+      <c r="B153" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="C151" s="27" t="s">
+      <c r="C153" s="27" t="s">
         <v>312</v>
-      </c>
-      <c r="D151" s="73">
-        <v>0</v>
-      </c>
-      <c r="E151" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A152" s="26" t="s">
-        <v>258</v>
-      </c>
-      <c r="B152" s="27" t="s">
-        <v>332</v>
-      </c>
-      <c r="C152" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="D152" s="73">
-        <v>1</v>
-      </c>
-      <c r="E152" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A153" s="26" t="s">
-        <v>259</v>
-      </c>
-      <c r="B153" s="27" t="s">
-        <v>333</v>
-      </c>
-      <c r="C153" s="27" t="s">
-        <v>98</v>
       </c>
       <c r="D153" s="73">
         <v>0</v>
@@ -5302,237 +5748,279 @@
       <c r="E153" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F153" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="26" t="s">
-        <v>79</v>
+        <v>258</v>
       </c>
       <c r="B154" s="27" t="s">
-        <v>201</v>
+        <v>332</v>
       </c>
       <c r="C154" s="27" t="s">
         <v>103</v>
       </c>
       <c r="D154" s="73">
+        <v>1</v>
+      </c>
+      <c r="E154" s="39">
+        <v>1</v>
+      </c>
+      <c r="F154" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="B155" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="C155" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D155" s="73">
+        <v>0</v>
+      </c>
+      <c r="E155" s="39">
+        <v>0</v>
+      </c>
+      <c r="F155" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B156" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="C156" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D156" s="73">
         <v>0.4</v>
       </c>
-      <c r="E154" s="39">
+      <c r="E156" s="39">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A155" s="34" t="s">
+      <c r="F156" s="39">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="B155" s="35" t="s">
+      <c r="B157" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="C155" s="35" t="s">
+      <c r="C157" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="D155" s="58">
+      <c r="D157" s="58">
         <v>3.2100000000000002E-6</v>
       </c>
-      <c r="E155" s="41">
+      <c r="E157" s="41">
         <v>2.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A156" s="34" t="s">
+      <c r="F157" s="41">
+        <v>2.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="B156" s="35" t="s">
+      <c r="B158" s="35" t="s">
         <v>334</v>
       </c>
-      <c r="C156" s="35" t="s">
+      <c r="C158" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="D156" s="74">
+      <c r="D158" s="74">
         <v>25</v>
       </c>
-      <c r="E156" s="39">
+      <c r="E158" s="39">
         <v>25</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A157" s="34" t="s">
+      <c r="F158" s="39">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="B157" s="35" t="s">
+      <c r="B159" s="35" t="s">
         <v>335</v>
       </c>
-      <c r="C157" s="35" t="s">
+      <c r="C159" s="35" t="s">
         <v>312</v>
       </c>
-      <c r="D157" s="74">
+      <c r="D159" s="74">
         <v>0</v>
       </c>
-      <c r="E157" s="39">
+      <c r="E159" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A158" s="34" t="s">
+      <c r="F159" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="B158" s="35" t="s">
+      <c r="B160" s="35" t="s">
         <v>336</v>
       </c>
-      <c r="C158" s="35" t="s">
+      <c r="C160" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="D158" s="74">
+      <c r="D160" s="74">
         <v>3.98</v>
       </c>
-      <c r="E158" s="39">
+      <c r="E160" s="39">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A159" s="34" t="s">
+      <c r="F160" s="39">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" s="34" t="s">
         <v>263</v>
       </c>
-      <c r="B159" s="35" t="s">
+      <c r="B161" s="35" t="s">
         <v>337</v>
       </c>
-      <c r="C159" s="35" t="s">
+      <c r="C161" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D159" s="74">
+      <c r="D161" s="74">
         <v>1</v>
       </c>
-      <c r="E159" s="39">
+      <c r="E161" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A160" s="34" t="s">
+      <c r="F161" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B160" s="35" t="s">
+      <c r="B162" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="C160" s="35" t="s">
+      <c r="C162" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="D160" s="58">
+      <c r="D162" s="58">
         <v>1.6666666666666666E-4</v>
       </c>
-      <c r="E160" s="40">
+      <c r="E162" s="40">
         <v>1.6666666666666666E-4</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A161" s="12" t="s">
+      <c r="F162" s="40">
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="B161" s="13" t="s">
+      <c r="B163" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="C161" s="13" t="s">
+      <c r="C163" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="D161" s="53">
+      <c r="D163" s="53">
         <v>1E-8</v>
       </c>
-      <c r="E161" s="41">
+      <c r="E163" s="41">
         <v>1E-8</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A162" s="12" t="s">
+      <c r="F163" s="41">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="B162" s="13" t="s">
+      <c r="B164" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="C162" s="13" t="s">
+      <c r="C164" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D162" s="66">
+      <c r="D164" s="66">
         <v>20</v>
       </c>
-      <c r="E162" s="39">
+      <c r="E164" s="39">
         <v>20</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A163" s="12" t="s">
+      <c r="F164" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="B163" s="13" t="s">
+      <c r="B165" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="C163" s="13" t="s">
+      <c r="C165" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="D163" s="66">
+      <c r="D165" s="66">
         <v>0</v>
       </c>
-      <c r="E163" s="39">
+      <c r="E165" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A164" s="12" t="s">
+      <c r="F165" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="B164" s="13" t="s">
+      <c r="B166" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C164" s="13" t="s">
+      <c r="C166" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D164" s="66">
+      <c r="D166" s="66">
         <v>2</v>
       </c>
-      <c r="E164" s="39">
+      <c r="E166" s="39">
         <v>2</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A165" s="12" t="s">
+      <c r="F166" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="B165" s="13" t="s">
+      <c r="B167" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="C165" s="13" t="s">
+      <c r="C167" s="13" t="s">
         <v>98</v>
-      </c>
-      <c r="D165" s="66">
-        <v>1</v>
-      </c>
-      <c r="E165" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A166" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="B166" s="13" t="s">
-        <v>360</v>
-      </c>
-      <c r="C166" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="D166" s="53">
-        <v>8.3333333333333331E-5</v>
-      </c>
-      <c r="E166" s="40">
-        <v>8.3333333333333331E-5</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A167" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="B167" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="C167" s="13" t="s">
-        <v>103</v>
       </c>
       <c r="D167" s="66">
         <v>1</v>
@@ -5540,434 +6028,1092 @@
       <c r="E167" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A168" s="28" t="s">
+      <c r="F167" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="B168" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="C168" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="D168" s="53">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="E168" s="40">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="F168" s="40">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B169" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="C169" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D169" s="66">
+        <v>1</v>
+      </c>
+      <c r="E169" s="39">
+        <v>1</v>
+      </c>
+      <c r="F169" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170" s="28" t="s">
         <v>271</v>
       </c>
-      <c r="B168" s="29" t="s">
+      <c r="B170" s="29" t="s">
         <v>362</v>
       </c>
-      <c r="C168" s="29" t="s">
+      <c r="C170" s="29" t="s">
         <v>363</v>
       </c>
-      <c r="D168" s="59">
+      <c r="D170" s="59">
         <v>2.3533050791148895E-8</v>
       </c>
-      <c r="E168" s="39">
+      <c r="E170" s="39">
         <v>2.3533050791148899E-8</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A169" s="28" t="s">
+      <c r="F170" s="39">
+        <v>2.3533050791148899E-8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171" s="28" t="s">
         <v>272</v>
       </c>
-      <c r="B169" s="29" t="s">
+      <c r="B171" s="29" t="s">
         <v>344</v>
       </c>
-      <c r="C169" s="29" t="s">
+      <c r="C171" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="D169" s="75">
+      <c r="D171" s="75">
         <v>20</v>
       </c>
-      <c r="E169" s="39">
+      <c r="E171" s="39">
         <v>20</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A170" s="28" t="s">
+      <c r="F171" s="39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="B170" s="29" t="s">
+      <c r="B172" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="C170" s="29" t="s">
+      <c r="C172" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="D170" s="75">
+      <c r="D172" s="75">
         <v>-0.187</v>
       </c>
-      <c r="E170" s="39">
+      <c r="E172" s="39">
         <v>-0.187</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A171" s="28" t="s">
+      <c r="F172" s="39">
+        <v>-0.187</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="B171" s="29" t="s">
+      <c r="B173" s="29" t="s">
         <v>346</v>
       </c>
-      <c r="C171" s="29" t="s">
+      <c r="C173" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="D171" s="75">
+      <c r="D173" s="75">
         <v>2.48</v>
       </c>
-      <c r="E171" s="39">
+      <c r="E173" s="39">
         <v>2.48</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A172" s="28" t="s">
+      <c r="F173" s="39">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174" s="28" t="s">
         <v>275</v>
       </c>
-      <c r="B172" s="29" t="s">
+      <c r="B174" s="29" t="s">
         <v>347</v>
       </c>
-      <c r="C172" s="29" t="s">
+      <c r="C174" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="D172" s="75">
+      <c r="D174" s="75">
         <v>1</v>
       </c>
-      <c r="E172" s="39">
+      <c r="E174" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A173" s="28" t="s">
+      <c r="F174" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A175" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="B173" s="29" t="s">
+      <c r="B175" s="29" t="s">
         <v>364</v>
       </c>
-      <c r="C173" s="29" t="s">
+      <c r="C175" s="29" t="s">
         <v>365</v>
       </c>
-      <c r="D173" s="59">
+      <c r="D175" s="59">
         <v>6.1060227588121015E-4</v>
       </c>
-      <c r="E173" s="39">
+      <c r="E175" s="39">
         <v>6.1060227588121015E-4</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A174" s="24" t="s">
+      <c r="F175" s="39">
+        <v>6.1060227588121015E-4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="B174" s="25" t="s">
+      <c r="B176" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="C174" s="25" t="s">
+      <c r="C176" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="D174" s="56">
+      <c r="D176" s="56">
         <v>6.41E-9</v>
       </c>
-      <c r="E174" s="39">
+      <c r="E176" s="39">
         <v>3.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A175" s="24" t="s">
+      <c r="F176" s="39">
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177" s="24" t="s">
         <v>278</v>
       </c>
-      <c r="B175" s="25" t="s">
+      <c r="B177" s="25" t="s">
         <v>348</v>
       </c>
-      <c r="C175" s="25" t="s">
+      <c r="C177" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D175" s="69">
+      <c r="D177" s="69">
         <v>25</v>
       </c>
-      <c r="E175" s="39">
+      <c r="E177" s="39">
         <v>25</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A176" s="24" t="s">
+      <c r="F177" s="39">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178" s="24" t="s">
         <v>279</v>
       </c>
-      <c r="B176" s="25" t="s">
+      <c r="B178" s="25" t="s">
         <v>349</v>
       </c>
-      <c r="C176" s="25" t="s">
+      <c r="C178" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="D176" s="69">
+      <c r="D178" s="69">
         <v>0</v>
       </c>
-      <c r="E176" s="39">
+      <c r="E178" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A177" s="24" t="s">
+      <c r="F178" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="B177" s="25" t="s">
+      <c r="B179" s="25" t="s">
         <v>350</v>
       </c>
-      <c r="C177" s="25" t="s">
+      <c r="C179" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="D177" s="69">
+      <c r="D179" s="69">
         <v>3.98</v>
       </c>
-      <c r="E177" s="39">
+      <c r="E179" s="39">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A178" s="24" t="s">
+      <c r="F179" s="39">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="B178" s="25" t="s">
+      <c r="B180" s="25" t="s">
         <v>351</v>
       </c>
-      <c r="C178" s="25" t="s">
+      <c r="C180" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D178" s="69">
+      <c r="D180" s="69">
         <v>1</v>
       </c>
-      <c r="E178" s="39">
+      <c r="E180" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A179" s="24" t="s">
+      <c r="F180" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A181" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="B179" s="25" t="s">
+      <c r="B181" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="C179" s="25" t="s">
+      <c r="C181" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="D179" s="56">
+      <c r="D181" s="56">
         <v>8.3333333333333331E-5</v>
       </c>
-      <c r="E179" s="40">
+      <c r="E181" s="40">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A180" s="8" t="s">
+      <c r="F181" s="40">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A182" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="B180" s="9" t="s">
+      <c r="B182" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="C180" s="9" t="s">
+      <c r="C182" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="D180" s="50">
+      <c r="D182" s="50">
         <v>6.41E-9</v>
       </c>
-      <c r="E180" s="39">
+      <c r="E182" s="39">
         <v>3.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A181" s="8" t="s">
+      <c r="F182" s="39">
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A183" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="B181" s="9" t="s">
+      <c r="B183" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="C181" s="9" t="s">
+      <c r="C183" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D181" s="62">
+      <c r="D183" s="62">
         <v>25</v>
       </c>
-      <c r="E181" s="39">
+      <c r="E183" s="39">
         <v>25</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A182" s="8" t="s">
+      <c r="F183" s="39">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A184" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="B182" s="9" t="s">
+      <c r="B184" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="C182" s="9" t="s">
+      <c r="C184" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="D182" s="62">
+      <c r="D184" s="62">
         <v>0</v>
       </c>
-      <c r="E182" s="39">
+      <c r="E184" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A183" s="8" t="s">
+      <c r="F184" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A185" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="B183" s="9" t="s">
+      <c r="B185" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="C183" s="9" t="s">
+      <c r="C185" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D183" s="62">
+      <c r="D185" s="62">
         <v>3.98</v>
       </c>
-      <c r="E183" s="39">
+      <c r="E185" s="39">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A184" s="8" t="s">
+      <c r="F185" s="39">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A186" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="B184" s="9" t="s">
+      <c r="B186" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="C184" s="9" t="s">
+      <c r="C186" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D184" s="62">
+      <c r="D186" s="62">
         <v>1</v>
       </c>
-      <c r="E184" s="39">
+      <c r="E186" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A185" s="8" t="s">
+      <c r="F186" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A187" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="B185" s="9" t="s">
+      <c r="B187" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="C185" s="9" t="s">
+      <c r="C187" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="D185" s="50">
+      <c r="D187" s="50">
         <v>8.3333333333333331E-5</v>
       </c>
-      <c r="E185" s="40">
+      <c r="E187" s="40">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A186" s="30" t="s">
+      <c r="F187" s="40">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A188" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="B186" s="31" t="s">
+      <c r="B188" s="31" t="s">
         <v>367</v>
       </c>
-      <c r="C186" s="31" t="s">
+      <c r="C188" s="31" t="s">
         <v>368</v>
       </c>
-      <c r="D186" s="60">
+      <c r="D188" s="60">
         <v>3.205E-9</v>
       </c>
-      <c r="E186" s="39">
+      <c r="E188" s="39">
         <v>1.9999999999999999E-7</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A187" s="30" t="s">
+      <c r="F188" s="39">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A189" s="30" t="s">
         <v>290</v>
       </c>
-      <c r="B187" s="31" t="s">
+      <c r="B189" s="31" t="s">
         <v>356</v>
       </c>
-      <c r="C187" s="31" t="s">
+      <c r="C189" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D187" s="76">
+      <c r="D189" s="76">
         <v>25</v>
       </c>
-      <c r="E187" s="39">
+      <c r="E189" s="39">
         <v>25</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A188" s="30" t="s">
+      <c r="F189" s="39">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A190" s="30" t="s">
         <v>291</v>
       </c>
-      <c r="B188" s="31" t="s">
+      <c r="B190" s="31" t="s">
         <v>357</v>
       </c>
-      <c r="C188" s="31" t="s">
+      <c r="C190" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="D188" s="76">
+      <c r="D190" s="76">
         <v>0</v>
       </c>
-      <c r="E188" s="39">
+      <c r="E190" s="39">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A189" s="30" t="s">
+      <c r="F190" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191" s="30" t="s">
         <v>292</v>
       </c>
-      <c r="B189" s="31" t="s">
+      <c r="B191" s="31" t="s">
         <v>358</v>
       </c>
-      <c r="C189" s="31" t="s">
+      <c r="C191" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="D189" s="76">
+      <c r="D191" s="76">
         <v>3.98</v>
       </c>
-      <c r="E189" s="39">
+      <c r="E191" s="39">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A190" s="30" t="s">
+      <c r="F191" s="39">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A192" s="30" t="s">
         <v>293</v>
       </c>
-      <c r="B190" s="31" t="s">
+      <c r="B192" s="31" t="s">
         <v>359</v>
       </c>
-      <c r="C190" s="31" t="s">
+      <c r="C192" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="D190" s="76">
+      <c r="D192" s="76">
         <v>1</v>
       </c>
-      <c r="E190" s="39">
+      <c r="E192" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A191" s="30" t="s">
+      <c r="F192" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A193" s="30" t="s">
         <v>294</v>
       </c>
-      <c r="B191" s="31" t="s">
+      <c r="B193" s="31" t="s">
         <v>371</v>
       </c>
-      <c r="C191" s="31" t="s">
+      <c r="C193" s="31" t="s">
         <v>370</v>
       </c>
-      <c r="D191" s="60">
+      <c r="D193" s="60">
         <v>8.3333333333333331E-5</v>
       </c>
-      <c r="E191" s="40">
+      <c r="E193" s="40">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A192" s="32" t="s">
+      <c r="F193" s="40">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194" s="32" t="s">
         <v>372</v>
       </c>
-      <c r="B192" s="33" t="s">
+      <c r="B194" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="C192" s="33" t="s">
+      <c r="C194" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="D192" s="45" t="s">
+      <c r="D194" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="E192" s="41" t="s">
+      <c r="E194" s="41" t="s">
         <v>417</v>
       </c>
+      <c r="F194" s="41" t="s">
+        <v>417</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E149">
+  <conditionalFormatting sqref="E118">
+    <cfRule type="colorScale" priority="103">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E145">
+    <cfRule type="colorScale" priority="102">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E151">
+    <cfRule type="colorScale" priority="101">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E145">
+    <cfRule type="colorScale" priority="100">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E118">
+    <cfRule type="colorScale" priority="99">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E151">
+    <cfRule type="colorScale" priority="97">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E145">
+    <cfRule type="colorScale" priority="98">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E145">
+    <cfRule type="colorScale" priority="96">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E118">
+    <cfRule type="colorScale" priority="95">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E117">
+    <cfRule type="colorScale" priority="94">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E145">
+    <cfRule type="colorScale" priority="93">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E151">
+    <cfRule type="colorScale" priority="92">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E117">
+    <cfRule type="colorScale" priority="91">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E118">
+    <cfRule type="colorScale" priority="90">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E151">
+    <cfRule type="colorScale" priority="89">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E151">
+    <cfRule type="colorScale" priority="88">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E145">
+    <cfRule type="colorScale" priority="87">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E129">
+    <cfRule type="colorScale" priority="86">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E114:E115">
+    <cfRule type="colorScale" priority="85">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E151">
+    <cfRule type="colorScale" priority="84">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E145">
+    <cfRule type="colorScale" priority="83">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E151">
+    <cfRule type="colorScale" priority="82">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E151">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E145">
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E114:E115">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E129">
+    <cfRule type="colorScale" priority="78">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E129">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E145">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E151">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E116">
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E116">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E117">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E118">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F118">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F145">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F151">
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F145">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F118">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F151">
+    <cfRule type="colorScale" priority="63">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F145">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F145">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F118">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F117">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F145">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F151">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
@@ -5979,7 +7125,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E149">
+  <conditionalFormatting sqref="F117">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -5991,7 +7137,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E143">
+  <conditionalFormatting sqref="F118">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
@@ -6003,7 +7149,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E143">
+  <conditionalFormatting sqref="F151">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -6015,7 +7161,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E149">
+  <conditionalFormatting sqref="F151">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -6027,7 +7173,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E149">
+  <conditionalFormatting sqref="F145">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -6039,7 +7185,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E143">
+  <conditionalFormatting sqref="F129">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -6051,7 +7197,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E112">
+  <conditionalFormatting sqref="F114:F115">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -6063,7 +7209,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E113">
+  <conditionalFormatting sqref="F151">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -6075,7 +7221,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E127">
+  <conditionalFormatting sqref="F145">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -6087,7 +7233,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E113">
+  <conditionalFormatting sqref="F151">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -6099,7 +7245,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E112">
+  <conditionalFormatting sqref="F151">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -6111,7 +7257,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E149">
+  <conditionalFormatting sqref="F145">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -6123,7 +7269,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E143">
+  <conditionalFormatting sqref="F114:F115">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -6135,7 +7281,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E113">
+  <conditionalFormatting sqref="F129">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -6147,7 +7293,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E149">
+  <conditionalFormatting sqref="F7">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -6159,7 +7305,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E149">
+  <conditionalFormatting sqref="F129">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -6171,7 +7317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E143">
+  <conditionalFormatting sqref="F145">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -6183,7 +7329,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E112">
+  <conditionalFormatting sqref="F151">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -6195,7 +7341,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E113">
+  <conditionalFormatting sqref="F116">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -6207,7 +7353,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E127">
+  <conditionalFormatting sqref="F116">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -6219,7 +7365,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
+  <conditionalFormatting sqref="F117">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -6231,7 +7377,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E113">
+  <conditionalFormatting sqref="F118">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -6243,56 +7389,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E127">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E143">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E149">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E114">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E114">
-    <cfRule type="colorScale" priority="31">
+  <conditionalFormatting sqref="E112:F113">
+    <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>